<commit_message>
Updating with latest mortality data. December 2020 should be stable now.
</commit_message>
<xml_diff>
--- a/mortality_germany.xlsx
+++ b/mortality_germany.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\python\mortality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\python\mortality2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3EF0EE-FCB5-4F23-B67D-A86CDA2B61D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2798A14C-DBDC-4210-B9FC-DDA903A0E26B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{6D538B7F-7614-4F16-BC21-F50DCE0D8D3C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{6D538B7F-7614-4F16-BC21-F50DCE0D8D3C}"/>
   </bookViews>
   <sheets>
     <sheet name="1950-2019 monatlich" sheetId="2" r:id="rId1"/>
@@ -16838,8 +16838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10B3D665-3853-442C-B1A5-3DFBFB64AD96}">
   <dimension ref="A1:NC6"/>
   <sheetViews>
-    <sheetView topLeftCell="LS1" workbookViewId="0">
-      <selection activeCell="LS1" sqref="LS1"/>
+    <sheetView tabSelected="1" topLeftCell="LN1" workbookViewId="0">
+      <selection activeCell="MH9" sqref="MH9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -23362,91 +23362,99 @@
       <c r="LX6" s="8">
         <v>3049</v>
       </c>
-      <c r="LY6" s="8">
-        <v>2514.26129234069</v>
-      </c>
-      <c r="LZ6" s="8">
-        <v>2513.66954630185</v>
-      </c>
-      <c r="MA6" s="8">
-        <v>2513.07780026301</v>
-      </c>
-      <c r="MB6" s="8">
-        <v>2512.4860542241699</v>
-      </c>
-      <c r="MC6" s="8">
-        <v>2511.8943081853299</v>
-      </c>
-      <c r="MD6" s="8">
-        <v>2511.3025621464999</v>
-      </c>
-      <c r="ME6" s="8">
-        <v>2510.7108161076599</v>
-      </c>
-      <c r="MF6" s="8">
-        <v>2510.1190700688198</v>
-      </c>
-      <c r="MG6" s="8">
-        <v>2509.5273240299798</v>
-      </c>
-      <c r="MH6" s="8">
-        <v>2508.9355779911398</v>
-      </c>
-      <c r="MI6" s="8">
-        <v>2508.3438319523002</v>
-      </c>
-      <c r="MJ6" s="8">
-        <v>2507.7520859134602</v>
-      </c>
-      <c r="MK6" s="8">
-        <v>2507.1603398746201</v>
-      </c>
-      <c r="ML6" s="8">
-        <v>2506.5685938357801</v>
-      </c>
-      <c r="MM6" s="8">
-        <v>2505.9768477969401</v>
-      </c>
-      <c r="MN6" s="8">
-        <v>2505.3851017581001</v>
-      </c>
-      <c r="MO6" s="8">
-        <v>2504.79335571926</v>
-      </c>
-      <c r="MP6" s="8">
-        <v>2504.20160968043</v>
-      </c>
-      <c r="MQ6" s="8">
-        <v>2503.60986364159</v>
-      </c>
-      <c r="MR6" s="8">
-        <v>2503.01811760275</v>
-      </c>
-      <c r="MS6" s="8">
-        <v>2502.4263715639099</v>
-      </c>
-      <c r="MT6" s="8">
-        <v>2501.8346255250699</v>
-      </c>
-      <c r="MU6" s="8">
-        <v>2501.2428794862299</v>
-      </c>
-      <c r="MV6" s="8">
-        <v>2500.6511334473898</v>
-      </c>
-      <c r="MW6" s="8">
-        <v>2500.0593874085498</v>
-      </c>
-      <c r="MX6" s="8">
-        <v>2499.4676413697098</v>
-      </c>
-      <c r="MY6" s="8">
-        <v>2498.8758953308702</v>
-      </c>
-      <c r="MZ6" s="8"/>
-      <c r="NA6" s="8"/>
-      <c r="NB6" s="8"/>
-      <c r="NC6" s="8"/>
+      <c r="LY6" s="7">
+        <v>3243</v>
+      </c>
+      <c r="LZ6" s="7">
+        <v>3147</v>
+      </c>
+      <c r="MA6" s="7">
+        <v>3255</v>
+      </c>
+      <c r="MB6" s="7">
+        <v>3320</v>
+      </c>
+      <c r="MC6" s="7">
+        <v>3290</v>
+      </c>
+      <c r="MD6" s="7">
+        <v>3109</v>
+      </c>
+      <c r="ME6" s="7">
+        <v>3359</v>
+      </c>
+      <c r="MF6" s="7">
+        <v>3330</v>
+      </c>
+      <c r="MG6" s="7">
+        <v>3351</v>
+      </c>
+      <c r="MH6" s="7">
+        <v>3363</v>
+      </c>
+      <c r="MI6" s="7">
+        <v>3507</v>
+      </c>
+      <c r="MJ6" s="7">
+        <v>3374</v>
+      </c>
+      <c r="MK6" s="7">
+        <v>3386</v>
+      </c>
+      <c r="ML6" s="7">
+        <v>3455</v>
+      </c>
+      <c r="MM6" s="7">
+        <v>3442</v>
+      </c>
+      <c r="MN6" s="7">
+        <v>3506</v>
+      </c>
+      <c r="MO6" s="7">
+        <v>3540</v>
+      </c>
+      <c r="MP6" s="7">
+        <v>3533</v>
+      </c>
+      <c r="MQ6" s="7">
+        <v>3448</v>
+      </c>
+      <c r="MR6" s="7">
+        <v>3343</v>
+      </c>
+      <c r="MS6" s="7">
+        <v>3580</v>
+      </c>
+      <c r="MT6" s="7">
+        <v>3684</v>
+      </c>
+      <c r="MU6" s="7">
+        <v>3711</v>
+      </c>
+      <c r="MV6" s="7">
+        <v>3491</v>
+      </c>
+      <c r="MW6" s="7">
+        <v>3446</v>
+      </c>
+      <c r="MX6" s="7">
+        <v>3382</v>
+      </c>
+      <c r="MY6" s="7">
+        <v>3524</v>
+      </c>
+      <c r="MZ6" s="7">
+        <v>3733</v>
+      </c>
+      <c r="NA6" s="7">
+        <v>3645</v>
+      </c>
+      <c r="NB6" s="7">
+        <v>3661</v>
+      </c>
+      <c r="NC6" s="7">
+        <v>3449</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23457,7 +23465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB05E663-FF6C-497F-987B-981F544F0DB7}">
   <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>

</xml_diff>